<commit_message>
TIER2 and 3 classes commented, Excel parameter files added
</commit_message>
<xml_diff>
--- a/results/example2/CONSTANTS_excel.xlsx
+++ b/results/example2/CONSTANTS_excel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\kant\geo-geohyd-u1\sebaswe\work\CryoGrid2020_25\results\peat_suossjavri2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\CryoGrid\results\example2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
   <si>
     <t>CONST</t>
   </si>
@@ -273,6 +273,30 @@
   </si>
   <si>
     <t>residual_wc_clay</t>
+  </si>
+  <si>
+    <t>Darcy_friction_factor</t>
+  </si>
+  <si>
+    <t>rough-pipe regime</t>
+  </si>
+  <si>
+    <t>tortuosity_air</t>
+  </si>
+  <si>
+    <t>used in Carman Kozeny model</t>
+  </si>
+  <si>
+    <t>viscosity_air</t>
+  </si>
+  <si>
+    <t>[kg/(m sec)]</t>
+  </si>
+  <si>
+    <t>R_spec</t>
+  </si>
+  <si>
+    <t>[J/K kg]</t>
   </si>
 </sst>
 </file>
@@ -596,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,214 +919,258 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="B28">
-        <v>1005</v>
+        <v>287.05799999999999</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29">
+        <v>1005</v>
+      </c>
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>0.4</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31">
-        <v>273.14999999999998</v>
-      </c>
-      <c r="C31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <v>273.14999999999998</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>15</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>9.81</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>38</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.73E-5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>16</v>
       </c>
-      <c r="B34">
+      <c r="B36">
         <v>989.63</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>37</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>17</v>
       </c>
-      <c r="B35">
+      <c r="B37">
         <v>1.5</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" s="3">
-        <v>400</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B39" s="3">
-        <v>4.0599999999999996</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" s="3">
-        <v>0.65</v>
+        <v>4.0599999999999996</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="B41" s="3">
-        <v>1.49</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B42" s="3">
-        <v>2.31</v>
-      </c>
-      <c r="D42" t="s">
-        <v>76</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B43" s="3">
-        <v>2.5</v>
+        <v>2.31</v>
+      </c>
+      <c r="D43" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B44" s="3">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" s="3">
-        <v>1.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B46" s="3">
-        <v>1.25</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B47" s="3">
-        <v>1.292</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1.292</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>79</v>
-      </c>
-      <c r="B48" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>67</v>
       </c>
       <c r="B49" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B51" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B52" s="3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B56">
+        <v>0.1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57">
+        <v>2.5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>